<commit_message>
Can now read pdf files Add comments to an Excel cell (openpyxl) Some corrections: cell.is_empty is now a property, DEFAULT_TRANSFORMS instead of TRANSFORMS
</commit_message>
<xml_diff>
--- a/sheetparser/tests/test_table1.xlsx
+++ b/sheetparser/tests/test_table1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="0" windowWidth="2880" windowHeight="7860" activeTab="5"/>
+    <workbookView xWindow="3210" yWindow="0" windowWidth="2880" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -394,6 +394,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +701,7 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="B3" s="15">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -712,7 +715,7 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="B4" s="15">
         <v>2</v>
       </c>
       <c r="C4" t="s">
@@ -726,7 +729,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="15">
         <v>3</v>
       </c>
       <c r="C5" t="s">
@@ -739,8 +742,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+    </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -766,7 +772,7 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="15">
         <v>1</v>
       </c>
       <c r="C8" t="s">
@@ -792,7 +798,7 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="B9" s="15">
         <v>2</v>
       </c>
       <c r="C9" t="s">
@@ -818,7 +824,7 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="B10" s="15">
         <v>3</v>
       </c>
       <c r="C10" t="s">
@@ -845,6 +851,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -852,12 +859,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
@@ -871,7 +880,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -885,7 +894,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -899,7 +908,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="15">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -912,8 +921,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
@@ -927,7 +939,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="15">
         <v>1</v>
       </c>
       <c r="B7" t="s">
@@ -941,7 +953,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="15">
         <v>2</v>
       </c>
       <c r="B8" t="s">
@@ -955,7 +967,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="15">
         <v>3</v>
       </c>
       <c r="B9" t="s">
@@ -968,18 +980,22 @@
         <v>29</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+    </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="15" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="15" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1258,9 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1458,5 +1472,6 @@
     <mergeCell ref="D10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- added OrRange and AndRange to allow that several sheets or range be tested - unified fill color interface for xlrd and openpyxl - some bug fix - reviewed Workbook constructor
</commit_message>
<xml_diff>
--- a/sheetparser/tests/test_table1.xlsx
+++ b/sheetparser/tests/test_table1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="0" windowWidth="2880" windowHeight="7860"/>
+    <workbookView xWindow="4815" yWindow="0" windowWidth="2880" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -387,6 +387,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -394,9 +397,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,6 +491,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -526,6 +543,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -681,7 +715,7 @@
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +735,7 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -715,7 +749,7 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>2</v>
       </c>
       <c r="C4" t="s">
@@ -729,7 +763,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>3</v>
       </c>
       <c r="C5" t="s">
@@ -743,10 +777,10 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
+      <c r="B6" s="12"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -772,7 +806,7 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>1</v>
       </c>
       <c r="C8" t="s">
@@ -798,7 +832,7 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>2</v>
       </c>
       <c r="C9" t="s">
@@ -824,7 +858,7 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>3</v>
       </c>
       <c r="C10" t="s">
@@ -860,13 +894,13 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
@@ -880,7 +914,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -894,7 +928,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -908,7 +942,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -922,10 +956,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="12"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
@@ -939,7 +973,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="12">
         <v>1</v>
       </c>
       <c r="B7" t="s">
@@ -953,7 +987,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="12">
         <v>2</v>
       </c>
       <c r="B8" t="s">
@@ -967,7 +1001,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="12">
         <v>3</v>
       </c>
       <c r="B9" t="s">
@@ -981,15 +1015,15 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="12"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1087,11 +1121,11 @@
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="13">
         <v>2017</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1139,11 +1173,11 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="13">
         <v>2017</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1274,7 +1308,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1286,16 +1322,16 @@
       <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="14">
         <v>2017</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="J2" s="14" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="J2" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -1408,11 +1444,11 @@
       <c r="H8" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D11" s="11" t="s">

</xml_diff>

<commit_message>
- notion of VisibleRows - fixed Range names - backward compatibility: Workbook re_dct - fixed indexed color
</commit_message>
<xml_diff>
--- a/sheetparser/tests/test_table1.xlsx
+++ b/sheetparser/tests/test_table1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="0" windowWidth="2880" windowHeight="7860"/>
+    <workbookView xWindow="8025" yWindow="0" windowWidth="2880" windowHeight="7860" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>a</t>
   </si>
@@ -257,6 +258,45 @@
   </si>
   <si>
     <t>A more complex example</t>
+  </si>
+  <si>
+    <t>With hidden rows</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c4</t>
+  </si>
+  <si>
+    <t>And colors:</t>
+  </si>
+  <si>
+    <t>(200,201,202)</t>
+  </si>
+  <si>
+    <t>pattern</t>
+  </si>
+  <si>
+    <t>no color</t>
+  </si>
+  <si>
+    <t>{'theme':5}</t>
   </si>
 </sst>
 </file>
@@ -280,7 +320,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +331,23 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8C9CA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightVertical">
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
@@ -373,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -398,12 +455,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC8C9CA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -714,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1510,4 +1575,94 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- interpretation of dates and times in xlrd - registration of pdf files - or on many patterns - IgnoreIf - unit tests for all backends
</commit_message>
<xml_diff>
--- a/sheetparser/tests/test_table1.xlsx
+++ b/sheetparser/tests/test_table1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8025" yWindow="0" windowWidth="2880" windowHeight="7860" activeTab="6"/>
+    <workbookView xWindow="9630" yWindow="0" windowWidth="2880" windowHeight="7860" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
   <si>
     <t>a</t>
   </si>
@@ -297,6 +298,18 @@
   </si>
   <si>
     <t>{'theme':5}</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Float:</t>
+  </si>
+  <si>
+    <t>Int:</t>
+  </si>
+  <si>
+    <t>Time:</t>
   </si>
 </sst>
 </file>
@@ -430,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -446,6 +459,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -455,9 +471,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1186,11 +1201,11 @@
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="16">
         <v>2017</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1238,11 +1253,11 @@
       <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="16">
         <v>2017</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1387,16 +1402,16 @@
       <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="17">
         <v>2017</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="J2" s="15" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="J2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -1509,11 +1524,11 @@
       <c r="H8" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D11" s="11" t="s">
@@ -1581,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1599,13 +1614,13 @@
       <c r="E1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="15" t="s">
         <v>86</v>
       </c>
       <c r="J1" t="s">
@@ -1665,4 +1680,54 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="19">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="20">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>